<commit_message>
Expanded SheetTemplate for dynamic attributes
</commit_message>
<xml_diff>
--- a/budgeteer-report-exporter/test-mapping.xlsx
+++ b/budgeteer-report-exporter/test-mapping.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>{flag:warning1}</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>{test} - {foo}</t>
+  </si>
+  <si>
+    <t>{dynamic.name}</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A5:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,6 +498,9 @@
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>

</xml_diff>